<commit_message>
refacto folder and fix error poetry
</commit_message>
<xml_diff>
--- a/excel_files/users.xlsx
+++ b/excel_files/users.xlsx
@@ -28,22 +28,22 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>dolor ipsum cillum amet</t>
-  </si>
-  <si>
-    <t>cupidatat</t>
-  </si>
-  <si>
-    <t>exercitation dolor dolor laborum</t>
-  </si>
-  <si>
-    <t>sint voluptate aliquip esse dolore</t>
-  </si>
-  <si>
-    <t>eiusmod ut dolor Duis</t>
-  </si>
-  <si>
-    <t>aute ad amet labore nisi</t>
+    <t>Duis culpa</t>
+  </si>
+  <si>
+    <t>sint officia eiusmod nulla</t>
+  </si>
+  <si>
+    <t>dolore laboris</t>
+  </si>
+  <si>
+    <t>consectetur Ut voluptate et dolor</t>
+  </si>
+  <si>
+    <t>dolore ad eiusmod</t>
+  </si>
+  <si>
+    <t>voluptate</t>
   </si>
 </sst>
 </file>
@@ -429,10 +429,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>580863055</v>
+        <v>294902898</v>
       </c>
       <c r="D2">
-        <v>479421815</v>
+        <v>690495123</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -443,10 +443,10 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1302773901</v>
+        <v>-942386301</v>
       </c>
       <c r="D3">
-        <v>1556966237</v>
+        <v>-1157565972</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -457,10 +457,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1305873728</v>
+        <v>-1992719263</v>
       </c>
       <c r="D4">
-        <v>-1226003734</v>
+        <v>982097709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update poetry to uv
</commit_message>
<xml_diff>
--- a/excel_files/users.xlsx
+++ b/excel_files/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -28,22 +28,34 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Duis culpa</t>
-  </si>
-  <si>
-    <t>sint officia eiusmod nulla</t>
-  </si>
-  <si>
-    <t>dolore laboris</t>
-  </si>
-  <si>
-    <t>consectetur Ut voluptate et dolor</t>
-  </si>
-  <si>
-    <t>dolore ad eiusmod</t>
-  </si>
-  <si>
-    <t>voluptate</t>
+    <t>dolore quis consectetur</t>
+  </si>
+  <si>
+    <t>magna in voluptate quis</t>
+  </si>
+  <si>
+    <t>adipisicing eiusmod magna in Excepteur</t>
+  </si>
+  <si>
+    <t>fugiat</t>
+  </si>
+  <si>
+    <t>in velit nostrud Excepteur</t>
+  </si>
+  <si>
+    <t>voluptate dolor tempor</t>
+  </si>
+  <si>
+    <t>quis do ad velit aute</t>
+  </si>
+  <si>
+    <t>culpa minim</t>
+  </si>
+  <si>
+    <t>eiusmod</t>
+  </si>
+  <si>
+    <t>anim Ut do</t>
   </si>
 </sst>
 </file>
@@ -401,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,13 +438,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2">
-        <v>294902898</v>
+        <v>-1650109834</v>
       </c>
       <c r="D2">
-        <v>690495123</v>
+        <v>-1325551028</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -440,13 +452,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>-942386301</v>
+        <v>-504719199</v>
       </c>
       <c r="D3">
-        <v>-1157565972</v>
+        <v>1835153350</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -454,13 +466,41 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>-1992719263</v>
+        <v>-572649954</v>
       </c>
       <c r="D4">
-        <v>982097709</v>
+        <v>-478153369</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>-921315400</v>
+      </c>
+      <c r="D5">
+        <v>1150486065</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>-1400435088</v>
+      </c>
+      <c r="D6">
+        <v>-261493675</v>
       </c>
     </row>
   </sheetData>

</xml_diff>